<commit_message>
add the ccab in redirect-pipeline
</commit_message>
<xml_diff>
--- a/Project_Of_HardwareSystem_2022/2022秋硬件综合训练课设资料发布包/cpu21-riscv/RISC-V单周期硬布线控制器表达式自动生成（2022-8-19）.xlsx
+++ b/Project_Of_HardwareSystem_2022/2022秋硬件综合训练课设资料发布包/cpu21-riscv/RISC-V单周期硬布线控制器表达式自动生成（2022-8-19）.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HustProjects\Project_Of_HardwareSystem_2022\2022秋硬件综合训练课设资料发布包\cpu21-riscv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77A3B16-F637-4BF6-B0D9-C1071DB6DD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7F6473-A282-45D7-B8F4-BEE6097E8E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="125">
   <si>
     <t>#</t>
   </si>
@@ -956,6 +956,14 @@
   </si>
   <si>
     <t>BLTU</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
     <phoneticPr fontId="26" type="noConversion"/>
   </si>
 </sst>
@@ -2187,8 +2195,8 @@
   </sheetPr>
   <dimension ref="A1:AN62"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView topLeftCell="AE22" workbookViewId="0">
+      <selection activeCell="AH29" sqref="AH29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
@@ -2308,10 +2316,10 @@
         <v>122</v>
       </c>
       <c r="AG1" s="25" t="s">
-        <v>13</v>
+        <v>123</v>
       </c>
       <c r="AH1" s="25" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="AI1" s="25" t="s">
         <v>13</v>
@@ -4737,8 +4745,12 @@
       <c r="AD26" s="31"/>
       <c r="AE26" s="31"/>
       <c r="AF26" s="31"/>
-      <c r="AG26" s="36"/>
-      <c r="AH26" s="36"/>
+      <c r="AG26" s="36">
+        <v>1</v>
+      </c>
+      <c r="AH26" s="36">
+        <v>1</v>
+      </c>
       <c r="AI26" s="36"/>
       <c r="AJ26" s="36"/>
       <c r="AK26" s="36"/>
@@ -4834,8 +4846,12 @@
       <c r="AD27" s="57"/>
       <c r="AE27" s="57"/>
       <c r="AF27" s="57"/>
-      <c r="AG27" s="58"/>
-      <c r="AH27" s="58"/>
+      <c r="AG27" s="58">
+        <v>1</v>
+      </c>
+      <c r="AH27" s="58">
+        <v>1</v>
+      </c>
       <c r="AI27" s="58"/>
       <c r="AJ27" s="58"/>
       <c r="AK27" s="58"/>
@@ -4936,7 +4952,9 @@
       </c>
       <c r="AF28" s="31"/>
       <c r="AG28" s="36"/>
-      <c r="AH28" s="36"/>
+      <c r="AH28" s="36">
+        <v>1</v>
+      </c>
       <c r="AI28" s="36"/>
       <c r="AJ28" s="36"/>
       <c r="AK28" s="36"/>
@@ -5030,8 +5048,12 @@
       <c r="AF29" s="57">
         <v>1</v>
       </c>
-      <c r="AG29" s="58"/>
-      <c r="AH29" s="58"/>
+      <c r="AG29" s="58">
+        <v>1</v>
+      </c>
+      <c r="AH29" s="58">
+        <v>1</v>
+      </c>
       <c r="AI29" s="58"/>
       <c r="AJ29" s="58"/>
       <c r="AK29" s="58"/>
@@ -7496,9 +7518,9 @@
   </sheetPr>
   <dimension ref="A1:AX63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AG29" sqref="AG29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -7644,11 +7666,11 @@
       </c>
       <c r="AF1" s="25" t="str">
         <f>真值表!AG1</f>
-        <v>XXX</v>
+        <v>R1</v>
       </c>
       <c r="AG1" s="25" t="str">
         <f>真值表!AH1</f>
-        <v>XXX</v>
+        <v>R2</v>
       </c>
       <c r="AH1" s="25" t="str">
         <f>真值表!AI1</f>
@@ -11494,11 +11516,11 @@
       </c>
       <c r="AF26" s="24" t="str">
         <f>IF(真值表!AG26=1,$O26&amp;"+","")</f>
-        <v/>
+        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="AG26" s="24" t="str">
         <f>IF(真值表!AH26=1,$O26&amp;"+","")</f>
-        <v/>
+        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="AH26" s="24" t="str">
         <f>IF(真值表!AI26=1,$O26&amp;"+","")</f>
@@ -11648,11 +11670,11 @@
       </c>
       <c r="AF27" s="49" t="str">
         <f>IF(真值表!AG27=1,$O27&amp;"+","")</f>
-        <v/>
+        <v xml:space="preserve"> F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="AG27" s="49" t="str">
         <f>IF(真值表!AH27=1,$O27&amp;"+","")</f>
-        <v/>
+        <v xml:space="preserve"> F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="AH27" s="49" t="str">
         <f>IF(真值表!AI27=1,$O27&amp;"+","")</f>
@@ -11806,7 +11828,7 @@
       </c>
       <c r="AG28" s="24" t="str">
         <f>IF(真值表!AH28=1,$O28&amp;"+","")</f>
-        <v/>
+        <v>~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="AH28" s="24" t="str">
         <f>IF(真值表!AI28=1,$O28&amp;"+","")</f>
@@ -11956,11 +11978,11 @@
       </c>
       <c r="AF29" s="49" t="str">
         <f>IF(真值表!AG29=1,$O29&amp;"+","")</f>
-        <v/>
+        <v xml:space="preserve"> F14&amp; F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="AG29" s="49" t="str">
         <f>IF(真值表!AH29=1,$O29&amp;"+","")</f>
-        <v/>
+        <v xml:space="preserve"> F14&amp; F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="AH29" s="49" t="str">
         <f>IF(真值表!AI29=1,$O29&amp;"+","")</f>
@@ -16379,11 +16401,11 @@
       </c>
       <c r="AF58" s="30" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+ F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp; F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2</v>
       </c>
       <c r="AG58" s="30" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+ F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+ F14&amp; F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2</v>
       </c>
       <c r="AH58" s="30" t="str">
         <f t="shared" si="2"/>
@@ -16479,11 +16501,11 @@
       </c>
       <c r="AF59" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+ F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+ F14&amp; F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="AG59" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>~F30&amp;~F25&amp;~F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+ F30&amp;~F25&amp; F14&amp;~F13&amp; F12&amp;~OP6&amp; OP5&amp; OP4&amp;~OP3&amp;~OP2+~F14&amp;~F13&amp;~F12&amp;~OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+ F14&amp; F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="AH59" t="str">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
branch prediction is finishedgit add .!
</commit_message>
<xml_diff>
--- a/Project_Of_HardwareSystem_2022/2022秋硬件综合训练课设资料发布包/cpu21-riscv/RISC-V单周期硬布线控制器表达式自动生成（2022-8-19）.xlsx
+++ b/Project_Of_HardwareSystem_2022/2022秋硬件综合训练课设资料发布包/cpu21-riscv/RISC-V单周期硬布线控制器表达式自动生成（2022-8-19）.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HustProjects\Project_Of_HardwareSystem_2022\2022秋硬件综合训练课设资料发布包\cpu21-riscv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7F6473-A282-45D7-B8F4-BEE6097E8E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24E4165-F252-44B1-BC27-35A86D0739E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="127">
   <si>
     <t>#</t>
   </si>
@@ -964,6 +964,14 @@
   </si>
   <si>
     <t>R2</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
     <phoneticPr fontId="26" type="noConversion"/>
   </si>
 </sst>
@@ -2195,8 +2203,8 @@
   </sheetPr>
   <dimension ref="A1:AN62"/>
   <sheetViews>
-    <sheetView topLeftCell="AE22" workbookViewId="0">
-      <selection activeCell="AH29" sqref="AH29"/>
+    <sheetView topLeftCell="P2" workbookViewId="0">
+      <selection activeCell="AJ29" sqref="AJ29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
@@ -2322,10 +2330,10 @@
         <v>124</v>
       </c>
       <c r="AI1" s="25" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="AJ1" s="25" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="AK1" s="25" t="s">
         <v>13</v>
@@ -5055,7 +5063,9 @@
         <v>1</v>
       </c>
       <c r="AI29" s="58"/>
-      <c r="AJ29" s="58"/>
+      <c r="AJ29" s="58">
+        <v>1</v>
+      </c>
       <c r="AK29" s="58"/>
       <c r="AL29" s="58"/>
       <c r="AM29" s="58"/>
@@ -7520,7 +7530,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AG29" sqref="AG29"/>
+      <selection pane="bottomLeft" activeCell="AI58" sqref="AI58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -7674,11 +7684,11 @@
       </c>
       <c r="AH1" s="25" t="str">
         <f>真值表!AI1</f>
-        <v>XXX</v>
+        <v>I</v>
       </c>
       <c r="AI1" s="25" t="str">
         <f>真值表!AJ1</f>
-        <v>XXX</v>
+        <v>B</v>
       </c>
       <c r="AJ1" s="25" t="str">
         <f>真值表!AK1</f>
@@ -11990,7 +12000,7 @@
       </c>
       <c r="AI29" s="49" t="str">
         <f>IF(真值表!AJ29=1,$O29&amp;"+","")</f>
-        <v/>
+        <v xml:space="preserve"> F14&amp; F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="AJ29" s="49" t="str">
         <f>IF(真值表!AK29=1,$O29&amp;"+","")</f>
@@ -16413,7 +16423,7 @@
       </c>
       <c r="AI58" s="30" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v xml:space="preserve"> F14&amp; F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2</v>
       </c>
       <c r="AJ58" s="30" t="str">
         <f t="shared" si="2"/>
@@ -16513,7 +16523,7 @@
       </c>
       <c r="AI59" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v xml:space="preserve"> F14&amp; F13&amp;~F12&amp; OP6&amp; OP5&amp;~OP4&amp;~OP3&amp;~OP2+</v>
       </c>
       <c r="AJ59" t="str">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Start to finish HS teamwork
</commit_message>
<xml_diff>
--- a/Project_Of_HardwareSystem_2022/2022秋硬件综合训练课设资料发布包/cpu21-riscv/RISC-V单周期硬布线控制器表达式自动生成（2022-8-19）.xlsx
+++ b/Project_Of_HardwareSystem_2022/2022秋硬件综合训练课设资料发布包/cpu21-riscv/RISC-V单周期硬布线控制器表达式自动生成（2022-8-19）.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HustProjects\Project_Of_HardwareSystem_2022\2022秋硬件综合训练课设资料发布包\cpu21-riscv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProjects\HustProjects\Project_Of_HardwareSystem_2022\2022秋硬件综合训练课设资料发布包\cpu21-riscv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24E4165-F252-44B1-BC27-35A86D0739E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A3CBF4-DF01-4D02-9BF7-772041396655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4940" yWindow="4940" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="真值表" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="128">
   <si>
     <t>#</t>
   </si>
@@ -972,6 +972,10 @@
   </si>
   <si>
     <t>B</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>tu</t>
     <phoneticPr fontId="26" type="noConversion"/>
   </si>
 </sst>
@@ -2201,10 +2205,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39994506668294322"/>
   </sheetPr>
-  <dimension ref="A1:AN62"/>
+  <dimension ref="A1:AN69"/>
   <sheetViews>
-    <sheetView topLeftCell="P2" workbookViewId="0">
-      <selection activeCell="AJ29" sqref="AJ29"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="AC69" sqref="AC69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
@@ -7427,6 +7431,11 @@
       <c r="AM61" s="58"/>
     </row>
     <row r="62" spans="1:39" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="69" spans="29:29" x14ac:dyDescent="0.45">
+      <c r="AC69" s="26" t="s">
+        <v>127</v>
+      </c>
+    </row>
   </sheetData>
   <protectedRanges>
     <protectedRange sqref="A1:E1048576" name="区域1" securityDescriptor=""/>
@@ -7528,7 +7537,7 @@
   </sheetPr>
   <dimension ref="A1:AX63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+    <sheetView topLeftCell="AA1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AI58" sqref="AI58"/>
     </sheetView>

</xml_diff>